<commit_message>
changes and added passport field
</commit_message>
<xml_diff>
--- a/public/sample_excel/candidate-example.xlsx
+++ b/public/sample_excel/candidate-example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
   <si>
     <t>mode_of_registration</t>
   </si>
@@ -81,9 +81,6 @@
     <t>return</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>indian_exp</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Junior Developer</t>
-  </si>
-  <si>
     <t>1 Year Experience</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>jolly@yopmail.com</t>
   </si>
   <si>
-    <t>mohon@yopmail.com</t>
-  </si>
-  <si>
     <t>ENCR</t>
   </si>
   <si>
@@ -220,6 +211,54 @@
   </si>
   <si>
     <t>BBA</t>
+  </si>
+  <si>
+    <t>position_applied_for_1</t>
+  </si>
+  <si>
+    <t>position_applied_for_2</t>
+  </si>
+  <si>
+    <t>position_applied_for_3</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT TALLY</t>
+  </si>
+  <si>
+    <t>ALUMINIUM FABRICATOR</t>
+  </si>
+  <si>
+    <t>ANIMAL WARDEN</t>
+  </si>
+  <si>
+    <t>ANY HELPER</t>
+  </si>
+  <si>
+    <t>ARBIC CHEF</t>
+  </si>
+  <si>
+    <t>AREA RESTURANT MANAGER</t>
+  </si>
+  <si>
+    <t>ARGON WELDER</t>
+  </si>
+  <si>
+    <t>ASST. COOK</t>
+  </si>
+  <si>
+    <t>ASST. COOK TANDOOR</t>
+  </si>
+  <si>
+    <t>ASST. ELECTRICIAN</t>
+  </si>
+  <si>
+    <t>ASST. INDIAN COOK</t>
+  </si>
+  <si>
+    <t>das@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -579,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,11 +640,13 @@
     <col min="19" max="19" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="22" customWidth="1"/>
+    <col min="25" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,45 +711,51 @@
         <v>20</v>
       </c>
       <c r="V1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J2">
         <v>8523456056</v>
@@ -717,75 +764,81 @@
         <v>5242525555</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2">
         <v>7485758586</v>
       </c>
       <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
       <c r="S2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" t="s">
         <v>36</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
         <v>37</v>
       </c>
-      <c r="W2" t="s">
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="X2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3">
         <v>8003456856</v>
@@ -794,75 +847,81 @@
         <v>5242525555</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M3">
         <v>7485758587</v>
       </c>
       <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
       <c r="P3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" t="s">
+        <v>69</v>
+      </c>
+      <c r="W3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
         <v>49</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>52</v>
       </c>
       <c r="J4">
         <v>8523006856</v>
@@ -871,75 +930,81 @@
         <v>5242525555</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M4">
         <v>7485758588</v>
       </c>
       <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
         <v>30</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>33</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" t="s">
         <v>34</v>
       </c>
-      <c r="S4" t="s">
-        <v>43</v>
-      </c>
-      <c r="T4" t="s">
-        <v>35</v>
-      </c>
       <c r="U4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" t="s">
+        <v>74</v>
+      </c>
+      <c r="X4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" t="s">
         <v>37</v>
       </c>
-      <c r="W4" t="s">
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="X4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5">
         <v>8523450000</v>
@@ -948,46 +1013,52 @@
         <v>5242525555</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="M5">
         <v>7485758589</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
         <v>33</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>34</v>
       </c>
-      <c r="S5" t="s">
-        <v>35</v>
-      </c>
       <c r="T5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="U5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V5" t="s">
+        <v>71</v>
+      </c>
+      <c r="W5" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" t="s">
         <v>37</v>
-      </c>
-      <c r="W5" t="s">
-        <v>38</v>
-      </c>
-      <c r="X5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
today's client changes 2
</commit_message>
<xml_diff>
--- a/public/sample_excel/candidate-example.xlsx
+++ b/public/sample_excel/candidate-example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>mode_of_registration</t>
   </si>
@@ -90,9 +90,6 @@
     <t>remark</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>BSC</t>
   </si>
   <si>
-    <t>john@yopmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kokata </t>
   </si>
   <si>
@@ -150,12 +144,6 @@
     <t>Poor</t>
   </si>
   <si>
-    <t>joy@yopmail.com</t>
-  </si>
-  <si>
-    <t>jolly@yopmail.com</t>
-  </si>
-  <si>
     <t>ENCR</t>
   </si>
   <si>
@@ -168,15 +156,6 @@
     <t>B.Tech</t>
   </si>
   <si>
-    <t>Joydeb Debnath</t>
-  </si>
-  <si>
-    <t>Jolly Bond</t>
-  </si>
-  <si>
-    <t>Mohon SK</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -222,45 +201,9 @@
     <t>position_applied_for_3</t>
   </si>
   <si>
-    <t>ACCOUNTANT</t>
-  </si>
-  <si>
-    <t>ACCOUNTANT TALLY</t>
-  </si>
-  <si>
-    <t>ALUMINIUM FABRICATOR</t>
-  </si>
-  <si>
-    <t>ANIMAL WARDEN</t>
-  </si>
-  <si>
-    <t>ANY HELPER</t>
-  </si>
-  <si>
-    <t>ARBIC CHEF</t>
-  </si>
-  <si>
     <t>AREA RESTURANT MANAGER</t>
   </si>
   <si>
-    <t>ARGON WELDER</t>
-  </si>
-  <si>
-    <t>ASST. COOK</t>
-  </si>
-  <si>
-    <t>ASST. COOK TANDOOR</t>
-  </si>
-  <si>
-    <t>ASST. ELECTRICIAN</t>
-  </si>
-  <si>
-    <t>ASST. INDIAN COOK</t>
-  </si>
-  <si>
-    <t>das@yopmail.com</t>
-  </si>
-  <si>
     <t>passport_number</t>
   </si>
   <si>
@@ -274,6 +217,69 @@
   </si>
   <si>
     <t>Z8575856</t>
+  </si>
+  <si>
+    <t>MACHINE EMBROIDER</t>
+  </si>
+  <si>
+    <t>MECHANICAL SUPERVISOR</t>
+  </si>
+  <si>
+    <t>MOBILE CRANE OPERATOR</t>
+  </si>
+  <si>
+    <t>OFFICE BOY</t>
+  </si>
+  <si>
+    <t>OFFICE MACHINE OPERATOR</t>
+  </si>
+  <si>
+    <t>LMV MECHANIC PETROL</t>
+  </si>
+  <si>
+    <t>FINISHING CARPENTER</t>
+  </si>
+  <si>
+    <t>GARDENER</t>
+  </si>
+  <si>
+    <t>WELDER</t>
+  </si>
+  <si>
+    <t>GENTS TAILOR</t>
+  </si>
+  <si>
+    <t>GLASS DESIGNER</t>
+  </si>
+  <si>
+    <t>Dinesh Kartick</t>
+  </si>
+  <si>
+    <t>Bipul Das</t>
+  </si>
+  <si>
+    <t>Nirmal Ghosh</t>
+  </si>
+  <si>
+    <t>Jahiralom Sk</t>
+  </si>
+  <si>
+    <t>dinesh@yopmail.com</t>
+  </si>
+  <si>
+    <t>bipul@yopmail.com</t>
+  </si>
+  <si>
+    <t>nirmal@yopmail.com</t>
+  </si>
+  <si>
+    <t>jahiralom@yopmail.com</t>
+  </si>
+  <si>
+    <t>Subham Ghosh</t>
+  </si>
+  <si>
+    <t>Dilip Ghosh</t>
   </si>
 </sst>
 </file>
@@ -635,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,13 +656,13 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
     <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.7109375" customWidth="1"/>
     <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="22" customWidth="1"/>
     <col min="26" max="27" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -724,19 +730,19 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="V1" t="s">
         <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="X1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="Y1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="Z1" t="s">
         <v>21</v>
@@ -750,346 +756,346 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J2">
-        <v>8523456056</v>
+        <v>7410258900</v>
       </c>
       <c r="K2">
         <v>5242525555</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2">
+        <v>917485758585</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="M2">
-        <v>7485758586</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" t="s">
         <v>35</v>
-      </c>
-      <c r="W2" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3">
-        <v>8003456856</v>
+        <v>8527418520</v>
       </c>
       <c r="K3">
         <v>5242525555</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="M3">
-        <v>7485758587</v>
+        <v>917485857585</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" t="s">
         <v>30</v>
       </c>
-      <c r="P3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>32</v>
-      </c>
       <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V3" t="s">
         <v>33</v>
       </c>
-      <c r="S3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" t="s">
         <v>35</v>
-      </c>
-      <c r="W3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J4">
-        <v>8523006856</v>
+        <v>9517539620</v>
       </c>
       <c r="K4">
         <v>5242525555</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="M4">
-        <v>7485758588</v>
+        <v>917485235695</v>
       </c>
       <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
         <v>29</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>30</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" t="s">
         <v>32</v>
       </c>
-      <c r="R4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" t="s">
-        <v>41</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" t="s">
+        <v>69</v>
+      </c>
+      <c r="X4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z4" t="s">
         <v>34</v>
       </c>
-      <c r="U4" t="s">
-        <v>84</v>
-      </c>
-      <c r="V4" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" t="s">
-        <v>70</v>
-      </c>
-      <c r="X4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>36</v>
-      </c>
       <c r="AA4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AB4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" t="s">
-        <v>64</v>
-      </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5">
-        <v>8523450000</v>
+        <v>8545632102</v>
       </c>
       <c r="K5">
         <v>5242525555</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="M5">
-        <v>7485758589</v>
+        <v>917485230230</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" t="s">
         <v>32</v>
       </c>
-      <c r="R5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" t="s">
+        <v>66</v>
+      </c>
+      <c r="V5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5" t="s">
+        <v>70</v>
+      </c>
+      <c r="X5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z5" t="s">
         <v>34</v>
       </c>
-      <c r="T5" t="s">
-        <v>41</v>
-      </c>
-      <c r="U5" t="s">
-        <v>85</v>
-      </c>
-      <c r="V5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" t="s">
-        <v>71</v>
-      </c>
-      <c r="X5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>36</v>
-      </c>
       <c r="AA5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AB5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implement base master layout for the application, including core HTML structure, CSS/JS imports, and modal definitions.
</commit_message>
<xml_diff>
--- a/public/sample_excel/candidate-example.xlsx
+++ b/public/sample_excel/candidate-example.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Al-hiraa\public\sample_excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -304,14 +309,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,338 +340,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -680,249 +357,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -930,64 +368,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1274,38 +669,38 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O5:T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5740740740741" customWidth="1"/>
-    <col min="3" max="3" width="11.5740740740741" customWidth="1"/>
-    <col min="4" max="4" width="19.5740740740741" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="7" max="7" width="10.4259259259259" customWidth="1"/>
-    <col min="8" max="8" width="15.4259259259259" customWidth="1"/>
-    <col min="9" max="9" width="15.8518518518519" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="20.1388888888889" customWidth="1"/>
-    <col min="13" max="14" width="21.8518518518519" customWidth="1"/>
-    <col min="19" max="19" width="21.4259259259259" customWidth="1"/>
-    <col min="20" max="20" width="27.5740740740741" customWidth="1"/>
-    <col min="21" max="22" width="13.712962962963" customWidth="1"/>
-    <col min="23" max="23" width="12.4259259259259" customWidth="1"/>
-    <col min="24" max="24" width="24.5740740740741" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="14" width="21.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" customWidth="1"/>
+    <col min="20" max="20" width="27.5703125" customWidth="1"/>
+    <col min="21" max="22" width="13.7109375" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="24.5703125" customWidth="1"/>
     <col min="25" max="26" width="22" customWidth="1"/>
-    <col min="27" max="28" width="16.712962962963" customWidth="1"/>
-    <col min="29" max="29" width="11.4259259259259" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -1435,7 +830,7 @@
         <v>38</v>
       </c>
       <c r="M2">
-        <v>917485758585</v>
+        <v>7485758585</v>
       </c>
       <c r="N2" t="s">
         <v>39</v>
@@ -1524,7 +919,7 @@
         <v>60</v>
       </c>
       <c r="M3">
-        <v>917485857585</v>
+        <v>7485857585</v>
       </c>
       <c r="N3" t="s">
         <v>39</v>
@@ -1611,7 +1006,7 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4">
-        <v>917485235695</v>
+        <v>7485235695</v>
       </c>
       <c r="N4" t="s">
         <v>39</v>
@@ -1698,7 +1093,7 @@
       </c>
       <c r="L5" s="3"/>
       <c r="M5">
-        <v>917485230230</v>
+        <v>7485230230</v>
       </c>
       <c r="N5" t="s">
         <v>39</v>
@@ -1751,43 +1146,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" display="kk@yopmail.com" tooltip="mailto:kk@yopmail.com"/>
-    <hyperlink ref="L3" r:id="rId2" display="dk@yopmail.com" tooltip="mailto:dk@yopmail.com"/>
+    <hyperlink ref="L2" r:id="rId1" tooltip="mailto:kk@yopmail.com"/>
+    <hyperlink ref="L3" r:id="rId2" tooltip="mailto:dk@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add sample Excel file for candidates.
</commit_message>
<xml_diff>
--- a/public/sample_excel/candidate-example.xlsx
+++ b/public/sample_excel/candidate-example.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>mode_of_registration</t>
   </si>
@@ -123,30 +123,18 @@
     <t>remark</t>
   </si>
   <si>
-    <t>Calling</t>
-  </si>
-  <si>
     <t>Facebook</t>
   </si>
   <si>
-    <t>Subham 2 Ghosh</t>
-  </si>
-  <si>
     <t>4/4/2022</t>
   </si>
   <si>
     <t>Dinesh Kartick</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>4/4/1999</t>
   </si>
   <si>
-    <t>Higer Secondary</t>
-  </si>
-  <si>
     <t>BCA</t>
   </si>
   <si>
@@ -159,21 +147,9 @@
     <t xml:space="preserve">Kokata </t>
   </si>
   <si>
-    <t>Hindu</t>
-  </si>
-  <si>
     <t>ECR</t>
   </si>
   <si>
-    <t>Four Wheeler</t>
-  </si>
-  <si>
-    <t>Two Wheeler</t>
-  </si>
-  <si>
-    <t>Poor</t>
-  </si>
-  <si>
     <t>S5632328</t>
   </si>
   <si>
@@ -198,9 +174,6 @@
     <t>Instagram</t>
   </si>
   <si>
-    <t>Azhar2 SK</t>
-  </si>
-  <si>
     <t>2022-04-04</t>
   </si>
   <si>
@@ -210,9 +183,6 @@
     <t>1998-10-10</t>
   </si>
   <si>
-    <t>MBA</t>
-  </si>
-  <si>
     <t>BSC</t>
   </si>
   <si>
@@ -222,9 +192,6 @@
     <t>ENCR</t>
   </si>
   <si>
-    <t>Basic</t>
-  </si>
-  <si>
     <t>P7418525</t>
   </si>
   <si>
@@ -240,18 +207,12 @@
     <t>Telecalling</t>
   </si>
   <si>
-    <t>Dilip2 Ghosh</t>
-  </si>
-  <si>
     <t>2021-04-04</t>
   </si>
   <si>
     <t>Nirmal Ghosh</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>1997-10-10</t>
   </si>
   <si>
@@ -261,9 +222,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>Y8575858</t>
   </si>
   <si>
@@ -276,9 +234,6 @@
     <t>WELDER</t>
   </si>
   <si>
-    <t>Azha2r SK</t>
-  </si>
-  <si>
     <t>2022-10-10</t>
   </si>
   <si>
@@ -288,12 +243,6 @@
     <t>1995-10-10</t>
   </si>
   <si>
-    <t>BBA</t>
-  </si>
-  <si>
-    <t>Muslim</t>
-  </si>
-  <si>
     <t>Z8575856</t>
   </si>
   <si>
@@ -304,6 +253,51 @@
   </si>
   <si>
     <t>GENTS TAILOR</t>
+  </si>
+  <si>
+    <t>HINDU</t>
+  </si>
+  <si>
+    <t>MUSLIM</t>
+  </si>
+  <si>
+    <t>CALLING</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>MASTERS</t>
+  </si>
+  <si>
+    <t>HIGHER SECONDARY</t>
+  </si>
+  <si>
+    <t>GRADUATES</t>
+  </si>
+  <si>
+    <t>4 WHEELER</t>
+  </si>
+  <si>
+    <t>2 WHEELER</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>POOR</t>
+  </si>
+  <si>
+    <t>BASIC</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>GOOD</t>
   </si>
 </sst>
 </file>
@@ -677,22 +671,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O5:T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="20.140625" customWidth="1"/>
     <col min="13" max="14" width="21.85546875" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.42578125" customWidth="1"/>
     <col min="20" max="20" width="27.5703125" customWidth="1"/>
     <col min="21" max="22" width="13.7109375" customWidth="1"/>
@@ -794,31 +791,28 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
       </c>
       <c r="J2">
         <v>7412258900</v>
@@ -827,87 +821,84 @@
         <v>5242525555</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M2">
         <v>7485758585</v>
       </c>
       <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" t="s">
+      <c r="X2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Y2" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Z2" t="s">
         <v>42</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AA2" t="s">
         <v>43</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AB2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC2" t="s">
         <v>44</v>
-      </c>
-      <c r="T2" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J3">
         <v>8555418520</v>
@@ -916,87 +907,84 @@
         <v>5242525555</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="M3">
         <v>7485857585</v>
       </c>
       <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" t="s">
+        <v>87</v>
+      </c>
+      <c r="V3" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="X3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA3" t="s">
         <v>43</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AB3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC3" t="s">
         <v>44</v>
-      </c>
-      <c r="T3" t="s">
-        <v>62</v>
-      </c>
-      <c r="U3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W3" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="J4">
         <v>9514439620</v>
@@ -1009,81 +997,78 @@
         <v>7485235695</v>
       </c>
       <c r="N4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="R4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" t="s">
+        <v>82</v>
+      </c>
+      <c r="T4" t="s">
+        <v>85</v>
+      </c>
+      <c r="U4" t="s">
+        <v>84</v>
+      </c>
+      <c r="V4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W4" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA4" t="s">
         <v>43</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AB4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC4" t="s">
         <v>44</v>
-      </c>
-      <c r="T4" t="s">
-        <v>74</v>
-      </c>
-      <c r="U4" t="s">
-        <v>75</v>
-      </c>
-      <c r="V4" t="s">
-        <v>76</v>
-      </c>
-      <c r="W4" t="s">
-        <v>74</v>
-      </c>
-      <c r="X4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
       <c r="I5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="J5">
         <v>8545222102</v>
@@ -1096,55 +1081,81 @@
         <v>7485230230</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="P5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" t="s">
+        <v>83</v>
+      </c>
+      <c r="T5" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" t="s">
         <v>85</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="V5" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" t="s">
         <v>61</v>
       </c>
-      <c r="R5" t="s">
+      <c r="X5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA5" t="s">
         <v>43</v>
       </c>
-      <c r="S5" t="s">
+      <c r="AB5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC5" t="s">
         <v>44</v>
-      </c>
-      <c r="T5" t="s">
-        <v>75</v>
-      </c>
-      <c r="U5" t="s">
-        <v>74</v>
-      </c>
-      <c r="V5" t="s">
-        <v>86</v>
-      </c>
-      <c r="W5" t="s">
-        <v>74</v>
-      </c>
-      <c r="X5" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576">
+      <formula1>"ECR,ECNR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576">
+      <formula1>"HINDU,MUSLIM,CHRISTIAN,SIKH,BUDDHIST,JAIN,OTHER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
+      <formula1>"CALLING,WALK-IN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>"MALE,FEMALE,OTHER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
+      <formula1>"5TH PASS,8TH PASS,10TH PASS,HIGHER SECONDARY,GRADUATES,MASTERS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:S1048576">
+      <formula1>"2 WHEELER,4 WHEELER,HV"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:U1048576">
+      <formula1>"BASIC,GOOD,POOR,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" tooltip="mailto:kk@yopmail.com"/>
     <hyperlink ref="L3" r:id="rId2" tooltip="mailto:dk@yopmail.com"/>

</xml_diff>